<commit_message>
Fix evaluation and activity log not showing up
</commit_message>
<xml_diff>
--- a/Activity Logs/Activity_Log.xlsx
+++ b/Activity Logs/Activity_Log.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>ACTIVITY LOG</t>
   </si>
@@ -66,6 +66,66 @@
   </si>
   <si>
     <t>Patrick Luis Francisco, MIT updated a grade record for student Test1 (18-0000) batch 2022.</t>
+  </si>
+  <si>
+    <t>Update Account</t>
+  </si>
+  <si>
+    <t>Patrick Luis Francisco, MIT updated their account information.</t>
+  </si>
+  <si>
+    <t>Export Evaluation Form</t>
+  </si>
+  <si>
+    <t>Patrick Luis Francisco, MIT exported an evaluation form for batch 2022, Department of Information Technology, First Semester and year level3.</t>
+  </si>
+  <si>
+    <t>Patrick Luis Francisco, MIT inserted a new record for student Student1 (18-0001) from the Department of Information Technology batch 2022.</t>
+  </si>
+  <si>
+    <t>Patrick Luis Francisco, MIT inserted a new grade record for student Student1 (18-0001) batch 2022.</t>
+  </si>
+  <si>
+    <t>Patrick Luis Francisco, MIT generated a report of grade record for student Student1 (18-0001).</t>
+  </si>
+  <si>
+    <t>Patrick Luis Francisco, MIT (ADMIN) login to the system.</t>
+  </si>
+  <si>
+    <t>Patrick Luis Francisco, MIT exported an evaluation form for batch 2022, Department of Information Technology, First Semester and year level2.</t>
+  </si>
+  <si>
+    <t>Patrick Luis Francisco, MIT inserted a new record for student student2 (18-0002) from the Department of Information Technology batch 2022.</t>
+  </si>
+  <si>
+    <t>Patrick Luis Francisco, MIT inserted a new grade record for student student2 (18-0002) batch 2022.</t>
+  </si>
+  <si>
+    <t>Patrick Luis Francisco, MIT generated a report for student student2 (18-0002).</t>
+  </si>
+  <si>
+    <t>Patrick Luis Francisco, MIT updated a grade record for student student2 (18-0002).</t>
+  </si>
+  <si>
+    <t>Patrick Luis Francisco, MIT exported an evaluation form for batch 2022, First Semester and year level2.</t>
+  </si>
+  <si>
+    <t>Patrick Luis Francisco, MIT exported an evaluation form for batch 2022, Second Semester and year level3.</t>
+  </si>
+  <si>
+    <t>Patrick Luis Francisco, MIT exported an evaluation form for batch 2022, First Semester and year level1.</t>
+  </si>
+  <si>
+    <t>Patrick Luis Francisco, MIT exported an evaluation form for batch 2022, Second Semester and year level2.</t>
+  </si>
+  <si>
+    <t>Patrick Luis Francisco, MIT inserted a new grade record for student Xeniorita Alondra L. Bio (18-0159) batch 2022.</t>
+  </si>
+  <si>
+    <t>Patrick Luis Francisco, MIT generated a report for student Xeniorita Alondra L. Bio (18-0159).</t>
+  </si>
+  <si>
+    <t>Patrick Luis Francisco, MIT updated a grade record for student Xeniorita Alondra L. Bio (18-0159).</t>
   </si>
 </sst>
 </file>
@@ -161,7 +221,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E89"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -304,47 +364,47 @@
     </row>
     <row r="9">
       <c r="A9" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="8">
-        <v>0.8590277777777777</v>
+        <v>0.8513888888888889</v>
       </c>
       <c r="C9" s="11">
-        <v>44710</v>
+        <v>44741</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="8">
-        <v>0.8597222222222223</v>
+        <v>0.8590277777777777</v>
       </c>
       <c r="C10" s="11">
-        <v>44711</v>
+        <v>44710</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="8">
-        <v>0.8625</v>
+        <v>0.8597222222222223</v>
       </c>
       <c r="C11" s="11">
-        <v>44712</v>
+        <v>44711</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>6</v>
@@ -355,10 +415,10 @@
     </row>
     <row r="12">
       <c r="A12" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="8">
-        <v>0.8631944444444445</v>
+        <v>0.8625</v>
       </c>
       <c r="C12" s="11">
         <v>44712</v>
@@ -372,13 +432,13 @@
     </row>
     <row r="13">
       <c r="A13" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="8">
-        <v>0.8638888888888889</v>
+        <v>0.8631944444444445</v>
       </c>
       <c r="C13" s="11">
-        <v>44713</v>
+        <v>44712</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>6</v>
@@ -389,10 +449,10 @@
     </row>
     <row r="14">
       <c r="A14" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="8">
-        <v>0.8736111111111111</v>
+        <v>0.8638888888888889</v>
       </c>
       <c r="C14" s="11">
         <v>44713</v>
@@ -402,6 +462,1281 @@
       </c>
       <c r="E14" s="6" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" s="8">
+        <v>0.8736111111111111</v>
+      </c>
+      <c r="C15" s="11">
+        <v>44713</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" s="8">
+        <v>0.8736111111111111</v>
+      </c>
+      <c r="C16" s="11">
+        <v>44717</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" s="8">
+        <v>0.9159722222222222</v>
+      </c>
+      <c r="C17" s="11">
+        <v>44717</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" s="8">
+        <v>0.9236111111111112</v>
+      </c>
+      <c r="C18" s="11">
+        <v>44717</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" s="8">
+        <v>0.9243055555555556</v>
+      </c>
+      <c r="C19" s="11">
+        <v>44717</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" s="8">
+        <v>0.9381944444444444</v>
+      </c>
+      <c r="C20" s="11">
+        <v>44717</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21" s="8">
+        <v>0.9395833333333333</v>
+      </c>
+      <c r="C21" s="11">
+        <v>44717</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22" s="8">
+        <v>0.9395833333333333</v>
+      </c>
+      <c r="C22" s="11">
+        <v>44717</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23" s="8">
+        <v>0.9402777777777778</v>
+      </c>
+      <c r="C23" s="11">
+        <v>44717</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24" s="8">
+        <v>0.9402777777777778</v>
+      </c>
+      <c r="C24" s="11">
+        <v>44717</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25" s="8">
+        <v>0.9416666666666667</v>
+      </c>
+      <c r="C25" s="11">
+        <v>44717</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26" s="8">
+        <v>0.9416666666666667</v>
+      </c>
+      <c r="C26" s="11">
+        <v>44717</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27" s="8">
+        <v>0.9451388888888889</v>
+      </c>
+      <c r="C27" s="11">
+        <v>44717</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1">
+        <v>26</v>
+      </c>
+      <c r="B28" s="8">
+        <v>0.9472222222222222</v>
+      </c>
+      <c r="C28" s="11">
+        <v>44717</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1">
+        <v>27</v>
+      </c>
+      <c r="B29" s="8">
+        <v>0.9493055555555555</v>
+      </c>
+      <c r="C29" s="11">
+        <v>44717</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1">
+        <v>28</v>
+      </c>
+      <c r="B30" s="8">
+        <v>0.95</v>
+      </c>
+      <c r="C30" s="11">
+        <v>44717</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="B31" s="8">
+        <v>0.9527777777777777</v>
+      </c>
+      <c r="C31" s="11">
+        <v>44717</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1">
+        <v>30</v>
+      </c>
+      <c r="B32" s="8">
+        <v>0.9534722222222223</v>
+      </c>
+      <c r="C32" s="11">
+        <v>44717</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1">
+        <v>31</v>
+      </c>
+      <c r="B33" s="8">
+        <v>0.9548611111111112</v>
+      </c>
+      <c r="C33" s="11">
+        <v>44717</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1">
+        <v>34</v>
+      </c>
+      <c r="B34" s="8">
+        <v>0.9638888888888889</v>
+      </c>
+      <c r="C34" s="11">
+        <v>44717</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1">
+        <v>35</v>
+      </c>
+      <c r="B35" s="8">
+        <v>0.9972222222222222</v>
+      </c>
+      <c r="C35" s="11">
+        <v>44717</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1">
+        <v>36</v>
+      </c>
+      <c r="B36" s="8">
+        <v>0.0125</v>
+      </c>
+      <c r="C36" s="11">
+        <v>44718</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1">
+        <v>37</v>
+      </c>
+      <c r="B37" s="8">
+        <v>0.015277777777777777</v>
+      </c>
+      <c r="C37" s="11">
+        <v>44718</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1">
+        <v>38</v>
+      </c>
+      <c r="B38" s="8">
+        <v>0.08333333333333333</v>
+      </c>
+      <c r="C38" s="11">
+        <v>44718</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1">
+        <v>39</v>
+      </c>
+      <c r="B39" s="8">
+        <v>0.0875</v>
+      </c>
+      <c r="C39" s="11">
+        <v>44718</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1">
+        <v>40</v>
+      </c>
+      <c r="B40" s="8">
+        <v>0.09097222222222222</v>
+      </c>
+      <c r="C40" s="11">
+        <v>44718</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1">
+        <v>41</v>
+      </c>
+      <c r="B41" s="8">
+        <v>0.09444444444444444</v>
+      </c>
+      <c r="C41" s="11">
+        <v>44718</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1">
+        <v>42</v>
+      </c>
+      <c r="B42" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="C42" s="11">
+        <v>44718</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1">
+        <v>43</v>
+      </c>
+      <c r="B43" s="8">
+        <v>0.10347222222222222</v>
+      </c>
+      <c r="C43" s="11">
+        <v>44718</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1">
+        <v>44</v>
+      </c>
+      <c r="B44" s="8">
+        <v>0.10625</v>
+      </c>
+      <c r="C44" s="11">
+        <v>44718</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1">
+        <v>45</v>
+      </c>
+      <c r="B45" s="8">
+        <v>0.1076388888888889</v>
+      </c>
+      <c r="C45" s="11">
+        <v>44718</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1">
+        <v>46</v>
+      </c>
+      <c r="B46" s="8">
+        <v>0.10972222222222222</v>
+      </c>
+      <c r="C46" s="11">
+        <v>44718</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1">
+        <v>47</v>
+      </c>
+      <c r="B47" s="8">
+        <v>0.1125</v>
+      </c>
+      <c r="C47" s="11">
+        <v>44718</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1">
+        <v>48</v>
+      </c>
+      <c r="B48" s="8">
+        <v>0.11597222222222223</v>
+      </c>
+      <c r="C48" s="11">
+        <v>44718</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1">
+        <v>49</v>
+      </c>
+      <c r="B49" s="8">
+        <v>0.11805555555555555</v>
+      </c>
+      <c r="C49" s="11">
+        <v>44718</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1">
+        <v>50</v>
+      </c>
+      <c r="B50" s="8">
+        <v>0.11875</v>
+      </c>
+      <c r="C50" s="11">
+        <v>44718</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E50" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1">
+        <v>51</v>
+      </c>
+      <c r="B51" s="8">
+        <v>0.12013888888888889</v>
+      </c>
+      <c r="C51" s="11">
+        <v>44718</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1">
+        <v>52</v>
+      </c>
+      <c r="B52" s="8">
+        <v>0.12569444444444444</v>
+      </c>
+      <c r="C52" s="11">
+        <v>44718</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1">
+        <v>53</v>
+      </c>
+      <c r="B53" s="8">
+        <v>0.12569444444444444</v>
+      </c>
+      <c r="C53" s="11">
+        <v>44718</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E53" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1">
+        <v>54</v>
+      </c>
+      <c r="B54" s="8">
+        <v>0.12986111111111112</v>
+      </c>
+      <c r="C54" s="11">
+        <v>44718</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E54" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1">
+        <v>55</v>
+      </c>
+      <c r="B55" s="8">
+        <v>0.13125</v>
+      </c>
+      <c r="C55" s="11">
+        <v>44718</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1">
+        <v>56</v>
+      </c>
+      <c r="B56" s="8">
+        <v>0.13194444444444445</v>
+      </c>
+      <c r="C56" s="11">
+        <v>44718</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E56" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1">
+        <v>57</v>
+      </c>
+      <c r="B57" s="8">
+        <v>0.13194444444444445</v>
+      </c>
+      <c r="C57" s="11">
+        <v>44718</v>
+      </c>
+      <c r="D57" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E57" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1">
+        <v>58</v>
+      </c>
+      <c r="B58" s="8">
+        <v>0.13194444444444445</v>
+      </c>
+      <c r="C58" s="11">
+        <v>44718</v>
+      </c>
+      <c r="D58" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E58" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1">
+        <v>59</v>
+      </c>
+      <c r="B59" s="8">
+        <v>0.1326388888888889</v>
+      </c>
+      <c r="C59" s="11">
+        <v>44718</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E59" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1">
+        <v>60</v>
+      </c>
+      <c r="B60" s="8">
+        <v>0.13402777777777777</v>
+      </c>
+      <c r="C60" s="11">
+        <v>44718</v>
+      </c>
+      <c r="D60" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E60" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1">
+        <v>61</v>
+      </c>
+      <c r="B61" s="8">
+        <v>0.13402777777777777</v>
+      </c>
+      <c r="C61" s="11">
+        <v>44718</v>
+      </c>
+      <c r="D61" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E61" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1">
+        <v>62</v>
+      </c>
+      <c r="B62" s="8">
+        <v>0.13472222222222222</v>
+      </c>
+      <c r="C62" s="11">
+        <v>44718</v>
+      </c>
+      <c r="D62" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E62" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1">
+        <v>63</v>
+      </c>
+      <c r="B63" s="8">
+        <v>0.13472222222222222</v>
+      </c>
+      <c r="C63" s="11">
+        <v>44718</v>
+      </c>
+      <c r="D63" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E63" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1">
+        <v>64</v>
+      </c>
+      <c r="B64" s="8">
+        <v>0.1375</v>
+      </c>
+      <c r="C64" s="11">
+        <v>44718</v>
+      </c>
+      <c r="D64" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E64" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1">
+        <v>65</v>
+      </c>
+      <c r="B65" s="8">
+        <v>0.1375</v>
+      </c>
+      <c r="C65" s="11">
+        <v>44718</v>
+      </c>
+      <c r="D65" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E65" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1">
+        <v>66</v>
+      </c>
+      <c r="B66" s="8">
+        <v>0.13819444444444445</v>
+      </c>
+      <c r="C66" s="11">
+        <v>44718</v>
+      </c>
+      <c r="D66" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E66" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1">
+        <v>67</v>
+      </c>
+      <c r="B67" s="8">
+        <v>0.13819444444444445</v>
+      </c>
+      <c r="C67" s="11">
+        <v>44718</v>
+      </c>
+      <c r="D67" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E67" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1">
+        <v>68</v>
+      </c>
+      <c r="B68" s="8">
+        <v>0.1388888888888889</v>
+      </c>
+      <c r="C68" s="11">
+        <v>44718</v>
+      </c>
+      <c r="D68" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E68" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1">
+        <v>69</v>
+      </c>
+      <c r="B69" s="8">
+        <v>0.14027777777777778</v>
+      </c>
+      <c r="C69" s="11">
+        <v>44718</v>
+      </c>
+      <c r="D69" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E69" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1">
+        <v>70</v>
+      </c>
+      <c r="B70" s="8">
+        <v>0.14027777777777778</v>
+      </c>
+      <c r="C70" s="11">
+        <v>44718</v>
+      </c>
+      <c r="D70" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E70" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1">
+        <v>71</v>
+      </c>
+      <c r="B71" s="8">
+        <v>0.21319444444444444</v>
+      </c>
+      <c r="C71" s="11">
+        <v>44718</v>
+      </c>
+      <c r="D71" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E71" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1">
+        <v>72</v>
+      </c>
+      <c r="B72" s="8">
+        <v>0.21388888888888888</v>
+      </c>
+      <c r="C72" s="11">
+        <v>44718</v>
+      </c>
+      <c r="D72" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E72" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1">
+        <v>73</v>
+      </c>
+      <c r="B73" s="8">
+        <v>0.21805555555555556</v>
+      </c>
+      <c r="C73" s="11">
+        <v>44718</v>
+      </c>
+      <c r="D73" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E73" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1">
+        <v>74</v>
+      </c>
+      <c r="B74" s="8">
+        <v>0.21875</v>
+      </c>
+      <c r="C74" s="11">
+        <v>44718</v>
+      </c>
+      <c r="D74" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E74" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1">
+        <v>75</v>
+      </c>
+      <c r="B75" s="8">
+        <v>0.22361111111111112</v>
+      </c>
+      <c r="C75" s="11">
+        <v>44718</v>
+      </c>
+      <c r="D75" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E75" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1">
+        <v>76</v>
+      </c>
+      <c r="B76" s="8">
+        <v>0.22361111111111112</v>
+      </c>
+      <c r="C76" s="11">
+        <v>44718</v>
+      </c>
+      <c r="D76" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E76" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1">
+        <v>77</v>
+      </c>
+      <c r="B77" s="8">
+        <v>0.2263888888888889</v>
+      </c>
+      <c r="C77" s="11">
+        <v>44718</v>
+      </c>
+      <c r="D77" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E77" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1">
+        <v>78</v>
+      </c>
+      <c r="B78" s="8">
+        <v>0.2263888888888889</v>
+      </c>
+      <c r="C78" s="11">
+        <v>44718</v>
+      </c>
+      <c r="D78" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E78" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1">
+        <v>79</v>
+      </c>
+      <c r="B79" s="8">
+        <v>0.23125</v>
+      </c>
+      <c r="C79" s="11">
+        <v>44718</v>
+      </c>
+      <c r="D79" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E79" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1">
+        <v>80</v>
+      </c>
+      <c r="B80" s="8">
+        <v>0.23125</v>
+      </c>
+      <c r="C80" s="11">
+        <v>44718</v>
+      </c>
+      <c r="D80" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E80" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1">
+        <v>81</v>
+      </c>
+      <c r="B81" s="8">
+        <v>0.23333333333333334</v>
+      </c>
+      <c r="C81" s="11">
+        <v>44718</v>
+      </c>
+      <c r="D81" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E81" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1">
+        <v>82</v>
+      </c>
+      <c r="B82" s="8">
+        <v>0.23402777777777778</v>
+      </c>
+      <c r="C82" s="11">
+        <v>44718</v>
+      </c>
+      <c r="D82" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E82" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1">
+        <v>83</v>
+      </c>
+      <c r="B83" s="8">
+        <v>0.2361111111111111</v>
+      </c>
+      <c r="C83" s="11">
+        <v>44718</v>
+      </c>
+      <c r="D83" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E83" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1">
+        <v>84</v>
+      </c>
+      <c r="B84" s="8">
+        <v>0.2548611111111111</v>
+      </c>
+      <c r="C84" s="11">
+        <v>44718</v>
+      </c>
+      <c r="D84" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E84" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1">
+        <v>85</v>
+      </c>
+      <c r="B85" s="8">
+        <v>0.2548611111111111</v>
+      </c>
+      <c r="C85" s="11">
+        <v>44718</v>
+      </c>
+      <c r="D85" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E85" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1">
+        <v>86</v>
+      </c>
+      <c r="B86" s="8">
+        <v>0.25555555555555554</v>
+      </c>
+      <c r="C86" s="11">
+        <v>44718</v>
+      </c>
+      <c r="D86" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E86" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1">
+        <v>87</v>
+      </c>
+      <c r="B87" s="8">
+        <v>0.25555555555555554</v>
+      </c>
+      <c r="C87" s="11">
+        <v>44718</v>
+      </c>
+      <c r="D87" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E87" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1">
+        <v>88</v>
+      </c>
+      <c r="B88" s="8">
+        <v>0.5243055555555556</v>
+      </c>
+      <c r="C88" s="11">
+        <v>44718</v>
+      </c>
+      <c r="D88" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E88" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="1">
+        <v>89</v>
+      </c>
+      <c r="B89" s="8">
+        <v>0.525</v>
+      </c>
+      <c r="C89" s="11">
+        <v>44718</v>
+      </c>
+      <c r="D89" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E89" s="6" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>